<commit_message>
PROS-9357 - CCRU - Check Visible Cooler KPI in Equipment Set for Petroleum REG
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/Contract Execution 2019.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/Contract Execution 2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MT - Hyper-Super" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="128">
   <si>
     <t xml:space="preserve">Action</t>
   </si>
@@ -401,9 +401,6 @@
   </si>
   <si>
     <t xml:space="preserve">PTR_2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,3</t>
   </si>
   <si>
     <t xml:space="preserve">PTR_2020</t>
@@ -782,7 +779,7 @@
   </sheetPr>
   <dimension ref="1:23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -795,30 +792,30 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="3" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="2" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="2" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="70.8056680161943"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="71.3400809716599"/>
     <col collapsed="false" hidden="false" max="33" min="32" style="4" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="36" min="34" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1023" min="37" style="2" width="9.10526315789474"/>
@@ -2437,30 +2434,30 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="3" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="2" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="2" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="72.7327935222672"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="73.3765182186235"/>
     <col collapsed="false" hidden="false" max="1023" min="32" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="8.57085020242915"/>
   </cols>
@@ -4060,28 +4057,28 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="5.35627530364372"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="2" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="3" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="2" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="2" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="70.8056680161943"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="71.3400809716599"/>
     <col collapsed="false" hidden="false" max="36" min="32" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1023" min="37" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="9.10526315789474"/>
@@ -4846,36 +4843,36 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="31.8137651821862"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="3" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="2" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="2" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="72.7327935222672"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="73.3765182186235"/>
     <col collapsed="false" hidden="false" max="36" min="32" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1023" min="37" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="8.57085020242915"/>
@@ -5701,8 +5698,8 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5716,28 +5713,28 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="5.35627530364372"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="3" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="2" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="2" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="70.8056680161943"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="71.3400809716599"/>
     <col collapsed="false" hidden="false" max="1023" min="32" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="9.10526315789474"/>
   </cols>
@@ -5981,7 +5978,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="11" t="s">
@@ -9136,7 +9133,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>43</v>
@@ -10192,7 +10189,7 @@
     </row>
     <row r="8" s="1" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="10" t="n">
         <v>7</v>
@@ -10211,7 +10208,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="11" t="s">
@@ -10335,7 +10332,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>79</v>
@@ -10345,7 +10342,7 @@
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O10" s="11" t="s">
         <v>50</v>
@@ -10410,7 +10407,7 @@
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>50</v>
@@ -10463,7 +10460,7 @@
         <v>5</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>79</v>
@@ -10473,7 +10470,7 @@
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O12" s="11" t="s">
         <v>50</v>
@@ -10520,7 +10517,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="11" t="s">
@@ -10927,30 +10924,30 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="31.8137651821862"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="69.0931174089069"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="69.7327935222672"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="53.3441295546559"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="53.7732793522267"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="3" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="2" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="2" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="2" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="72.7327935222672"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="73.3765182186235"/>
     <col collapsed="false" hidden="false" max="36" min="32" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1023" min="37" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="8.57085020242915"/>
@@ -11062,7 +11059,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>34</v>
@@ -11122,7 +11119,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>34</v>
@@ -11182,7 +11179,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>43</v>
@@ -11237,7 +11234,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>43</v>
@@ -11304,7 +11301,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>43</v>
@@ -11371,7 +11368,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>43</v>
@@ -11438,7 +11435,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>43</v>
@@ -11451,7 +11448,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="11" t="s">
@@ -11493,7 +11490,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>43</v>
@@ -11556,7 +11553,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>43</v>
@@ -11619,7 +11616,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>43</v>
@@ -11638,7 +11635,7 @@
         <v>5</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>79</v>
@@ -11648,7 +11645,7 @@
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>50</v>
@@ -11684,7 +11681,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>43</v>
@@ -11703,7 +11700,7 @@
         <v>5</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>79</v>
@@ -11713,7 +11710,7 @@
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O12" s="11" t="s">
         <v>50</v>
@@ -11749,7 +11746,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>43</v>
@@ -11768,7 +11765,7 @@
         <v>5</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>79</v>
@@ -11778,7 +11775,7 @@
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O13" s="11" t="s">
         <v>50</v>

</xml_diff>